<commit_message>
Added Maskinpark, PHP and Contact Changes
Added main section structure to maskinpark.html with styling. Copy and images needed to proceed.

Changed validation and functionality in mail.php,
Changed form structure in contact.html
contact.html and mail.php is still under development.
</commit_message>
<xml_diff>
--- a/documents/timeline.xlsx
+++ b/documents/timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubenhansen/OneDrive/front-end-developer/personal-projects/SenjaMaskinAS/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0dd4cf6328f227f/front-end-developer/personal-projects/SenjaMaskinAS/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{4363A934-C6EF-9D4F-9708-2CFD26DDF8B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{28392424-EB54-2E4B-A3AA-4E02A0BD5702}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="8_{4363A934-C6EF-9D4F-9708-2CFD26DDF8B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{0F38511C-13B2-D943-BF3D-A70E2AA5773C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{E75915D2-EAAF-1641-AF64-70E051B93E83}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Task 1</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>...</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -857,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E3C6D4-EF6F-4340-9CFF-BA80F76D7FCD}">
-  <dimension ref="B2:Y41"/>
+  <dimension ref="B2:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,10 +872,10 @@
     <col min="3" max="3" width="28.5" customWidth="1"/>
     <col min="4" max="5" width="9.5" customWidth="1"/>
     <col min="6" max="6" width="3.1640625" customWidth="1"/>
-    <col min="7" max="25" width="3.5" customWidth="1"/>
+    <col min="7" max="28" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" ht="65" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:28" ht="65" x14ac:dyDescent="0.2">
       <c r="G2" s="1">
         <v>43453</v>
       </c>
@@ -930,8 +933,17 @@
       <c r="Y2" s="1">
         <v>43492</v>
       </c>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="Z2" s="1">
+        <v>43493</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>43494</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>43495</v>
+      </c>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.2">
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -952,8 +964,11 @@
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+    </row>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -986,8 +1001,11 @@
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
-    </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1022,8 +1040,11 @@
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+    </row>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1066,8 +1087,11 @@
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1078,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="7"/>
@@ -1105,17 +1129,28 @@
         <v>3</v>
       </c>
       <c r="T7" s="7">
+        <v>3</v>
+      </c>
+      <c r="U7" s="7">
+        <v>3</v>
+      </c>
+      <c r="V7" s="7">
+        <v>3</v>
+      </c>
+      <c r="W7" s="7">
         <v>2</v>
       </c>
-      <c r="U7" s="7">
+      <c r="X7" s="7">
         <v>1</v>
       </c>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="Y7" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1145,17 +1180,20 @@
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
-      <c r="W8" s="7">
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7">
         <v>1</v>
       </c>
-      <c r="X8" s="7">
+      <c r="AA8" s="7">
         <v>1</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="AB8" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.2">
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1176,8 +1214,11 @@
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1230,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
@@ -1201,7 +1242,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1213,7 +1254,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
@@ -1225,7 +1266,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1389,7 +1430,7 @@
         <v>49</v>
       </c>
       <c r="D31" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" s="3"/>
     </row>
@@ -1401,10 +1442,10 @@
         <v>50</v>
       </c>
       <c r="D32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>46</v>
       </c>
@@ -1412,10 +1453,10 @@
         <v>51</v>
       </c>
       <c r="D33" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>47</v>
       </c>
@@ -1426,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>48</v>
       </c>
@@ -1436,8 +1477,11 @@
       <c r="D35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>54</v>
       </c>
@@ -1448,7 +1492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>3</v>
       </c>
@@ -1459,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>36</v>
       </c>
@@ -1470,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>37</v>
       </c>
@@ -1481,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>38</v>
       </c>
@@ -1493,7 +1537,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D5:D8 G7:H7 J7:L7 G5:L6 G8:L8 M5:Y8 E28:E31 D38:D41">
+  <conditionalFormatting sqref="D5:D8 G7:H7 J7:L7 G5:L6 G8:L8 E28:E31 D38:D41 M5:AB8">
     <cfRule type="containsText" dxfId="26" priority="37" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",D5)))</formula>
     </cfRule>

</xml_diff>